<commit_message>
updated excel row fetching method
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Username</t>
   </si>
@@ -40,12 +40,24 @@
   </si>
   <si>
     <t>Product</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -87,7 +99,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -100,6 +112,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -148,7 +163,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -181,9 +196,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -216,6 +248,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -395,7 +444,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,6 +471,9 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -430,13 +482,19 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2">
-        <v>123</v>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added getCellData in ReadExcel
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>C</t>
-  </si>
-  <si>
-    <t>123</t>
   </si>
 </sst>
 </file>
@@ -444,7 +441,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,8 +487,8 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
+      <c r="B4" s="2">
+        <v>123</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
End to end scenario with new test Data
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Username</t>
   </si>
@@ -30,31 +30,25 @@
     <t>Anushka19915</t>
   </si>
   <si>
-    <t>abc@abc.com</t>
-  </si>
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>123@113.com</t>
-  </si>
-  <si>
     <t>Product</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Cognizant</t>
+  </si>
+  <si>
+    <t>Noise Grey Knitted Slouchy Beanie</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -93,12 +87,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -160,7 +151,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -193,26 +184,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -245,23 +219,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -438,19 +395,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A4" activeCellId="1" sqref="A3:XFD3 A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,10 +416,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -471,34 +435,16 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2">
-        <v>123</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
inserted additional columns in the excel files
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Username</t>
   </si>
@@ -27,9 +27,6 @@
     <t>appumuv@gmail.com</t>
   </si>
   <si>
-    <t>Anushka19915</t>
-  </si>
-  <si>
     <t>Product</t>
   </si>
   <si>
@@ -42,7 +39,25 @@
     <t>Cognizant</t>
   </si>
   <si>
-    <t>Noise Grey Knitted Slouchy Beanie</t>
+    <t>Min Price</t>
+  </si>
+  <si>
+    <t>Max Price</t>
+  </si>
+  <si>
+    <t>Os</t>
+  </si>
+  <si>
+    <t>Android</t>
+  </si>
+  <si>
+    <t>num</t>
+  </si>
+  <si>
+    <t>Manik1591@#1</t>
+  </si>
+  <si>
+    <t>Mobiles</t>
   </si>
 </sst>
 </file>
@@ -395,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" activeCellId="1" sqref="A3:XFD3 A4:XFD4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,7 +423,7 @@
     <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -416,35 +431,60 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>5000</v>
+      </c>
+      <c r="G2">
+        <v>10000</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>